<commit_message>
Commit for sharing data
</commit_message>
<xml_diff>
--- a/data/CABG Hyperglycemia Variable List.xlsx
+++ b/data/CABG Hyperglycemia Variable List.xlsx
@@ -3,9 +3,10 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7647E3C7-C77D-432B-A35D-CC3BEBD2A9B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD455D0-CD13-4B6D-84B4-86EEDECD6849}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6640" firstSheet="3" activeTab="5" xr2:uid="{D77AD16B-127C-49C6-A7A9-A7B3BB10E535}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6640" firstSheet="3" activeTab="3" xr2:uid="{D77AD16B-127C-49C6-A7A9-A7B3BB10E535}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6640" firstSheet="3" activeTab="6" xr2:uid="{B96CC77E-FCF4-46B2-81D7-CEA310C0BD20}"/>
   </bookViews>
   <sheets>
     <sheet name="or_to_icu" sheetId="1" state="hidden" r:id="rId1"/>
@@ -14,9 +15,16 @@
     <sheet name="METACABG 20230706" sheetId="7" r:id="rId4"/>
     <sheet name="CGM Review" sheetId="9" r:id="rId5"/>
     <sheet name="METACABG CGM" sheetId="8" r:id="rId6"/>
-    <sheet name="cgm_summary" sheetId="3" r:id="rId7"/>
-    <sheet name="aha glucose" sheetId="5" state="hidden" r:id="rId8"/>
-    <sheet name="aha patient" sheetId="6" state="hidden" r:id="rId9"/>
+    <sheet name="bg_longitudinal" sheetId="10" r:id="rId7"/>
+    <sheet name="cgm_summary" sheetId="3" r:id="rId8"/>
+    <sheet name="cgm harmonization" sheetId="11" r:id="rId9"/>
+    <sheet name="cgm insertion dates" sheetId="12" r:id="rId10"/>
+    <sheet name="corrected key observation dates" sheetId="13" r:id="rId11"/>
+    <sheet name="insulinbolus_longitudinal" sheetId="14" r:id="rId12"/>
+    <sheet name="insulindrip_longitudinal" sheetId="15" r:id="rId13"/>
+    <sheet name="screening" sheetId="17" r:id="rId14"/>
+    <sheet name="aha glucose" sheetId="5" state="hidden" r:id="rId15"/>
+    <sheet name="aha patient" sheetId="6" state="hidden" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'METACABG 20230706'!$B$1:$I$505</definedName>
@@ -65,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3489" uniqueCount="2290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3613" uniqueCount="2346">
   <si>
     <t>variable</t>
   </si>
@@ -6997,6 +7005,174 @@
   </si>
   <si>
     <t xml:space="preserve">LGA 8/2/2023 added; MCM033 - CGM 1, sensor lost. Patient left with the sensor on, said he would return it but never did. </t>
+  </si>
+  <si>
+    <t>Unique patient ID</t>
+  </si>
+  <si>
+    <t>Date of surgery</t>
+  </si>
+  <si>
+    <t>Date of observation day 1</t>
+  </si>
+  <si>
+    <t>Date of observation day 2</t>
+  </si>
+  <si>
+    <t>Blinded group</t>
+  </si>
+  <si>
+    <t>Date of CGM1 insertion</t>
+  </si>
+  <si>
+    <t>Date of CGM2 insertion</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <t>sensorglucose</t>
+  </si>
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t>cgm_id</t>
+  </si>
+  <si>
+    <t>cgm_type</t>
+  </si>
+  <si>
+    <t>Timestamp in YYYY-MM-DD HH:MM:SS</t>
+  </si>
+  <si>
+    <t>Glucose in mg/dL</t>
+  </si>
+  <si>
+    <t>source file after initial cleaning located in [Smith, Ryan - Emory_Pasquel_F_CABG_Hyperglycemia\Glucose and Insulin Data\raw\CGM]</t>
+  </si>
+  <si>
+    <t>CGM identifier (internal)</t>
+  </si>
+  <si>
+    <t>CGM 1 or CGM 2?</t>
+  </si>
+  <si>
+    <t>Same as cgm1_status from CABG Hyperglycemia Variable List &gt;&gt; Sheet 'METACABG CGM'</t>
+  </si>
+  <si>
+    <t>date_event_name</t>
+  </si>
+  <si>
+    <t>Surgery or Post 1 or Post 2</t>
+  </si>
+  <si>
+    <t>Date of event_name for QC purposes</t>
+  </si>
+  <si>
+    <t>domain</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>date_measurement</t>
+  </si>
+  <si>
+    <t>or_bg [Blood glucose in OR] or cgmbg_bg [Blood glucose checked against CGM] or meal_bg [Blood glucose at time of meal]</t>
+  </si>
+  <si>
+    <t>serial number</t>
+  </si>
+  <si>
+    <t>Time in HH:MM:SS</t>
+  </si>
+  <si>
+    <t>Date of measurement</t>
+  </si>
+  <si>
+    <t>date_measurement + time</t>
+  </si>
+  <si>
+    <t>or_ibolus [Insulin bolus in OR] or icu48_isq [Insulin bolus in ICU]</t>
+  </si>
+  <si>
+    <t>Insulin units</t>
+  </si>
+  <si>
+    <t>time_start</t>
+  </si>
+  <si>
+    <t>time_stop</t>
+  </si>
+  <si>
+    <t>Time when drip started in HH:MM:SS</t>
+  </si>
+  <si>
+    <t>Time when drip stopped in HH:MM:SS</t>
+  </si>
+  <si>
+    <t>time_total</t>
+  </si>
+  <si>
+    <t>Time between time_start and time_stop in hours</t>
+  </si>
+  <si>
+    <t>rate_value</t>
+  </si>
+  <si>
+    <t>Insulin units (rate per hour)</t>
+  </si>
+  <si>
+    <t>units_value</t>
+  </si>
+  <si>
+    <t>Insulin units (total)</t>
+  </si>
+  <si>
+    <t>date_stop</t>
+  </si>
+  <si>
+    <t>timestamp_start</t>
+  </si>
+  <si>
+    <t>timestamp_stop</t>
+  </si>
+  <si>
+    <t>Usually same as date_measurement, except if drip was run overnight</t>
+  </si>
+  <si>
+    <t>Date of measurement (date of drip)</t>
+  </si>
+  <si>
+    <t>date_measurement + time_start</t>
+  </si>
+  <si>
+    <t>date_stop + time_stop</t>
+  </si>
+  <si>
+    <t>screening for everyone</t>
+  </si>
+  <si>
+    <t>Age at time of consent [ref: CABG Hyperglycemia Variable List &gt;&gt; Sheet 'METACABG 2023-0706')</t>
+  </si>
+  <si>
+    <t>Male or Female</t>
+  </si>
+  <si>
+    <t>Black or White or Hispanic or Other</t>
+  </si>
+  <si>
+    <t>Asian or 'NA'</t>
+  </si>
+  <si>
+    <t>BMI in kg/m2</t>
+  </si>
+  <si>
+    <t>Intervention or Observation Only? [ref: CABG Hyperglycemia Variable List &gt;&gt; Sheet 'METACABG 2023-0706')</t>
   </si>
 </sst>
 </file>
@@ -7453,6 +7629,7 @@
   <dimension ref="A1:C95"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -8251,11 +8428,1808 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D805C213-73B7-4BDA-9D53-9A17290325F0}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2290</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>2069</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2291</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>2070</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2292</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>2071</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2293</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2294</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2345</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>1302</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2295</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>1309</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2296</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF4A8C48-B656-4918-9751-2A06B95AB2C6}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2290</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>762</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2309</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>2308</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2310</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB2DA843-64A0-4D27-8FB3-0127EBCBA411}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="104.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2290</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>762</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2309</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>2311</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2320</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>2312</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2316</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>1482</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2317</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>2313</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2321</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>2314</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2318</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>2297</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2319</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40644621-1763-4A03-B26A-EAFD1B94CF35}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2290</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>762</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2309</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>2311</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2320</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>2312</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2316</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>2322</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2324</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>2323</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2325</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>2326</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2327</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>2328</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2329</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>2330</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>2314</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2336</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>2332</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2335</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>2333</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2337</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>2334</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2338</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB7DBC14-5454-4391-A166-41E8DEDC2E26}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2290</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>762</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2339</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2340</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>517</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2341</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>518</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2342</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2343</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2344</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2345</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F730E738-71E8-4BB9-9BDD-FAFBA3CE3EC3}">
+  <dimension ref="A1:B146"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="56.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>687</v>
+      </c>
+      <c r="B4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>685</v>
+      </c>
+      <c r="B5" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>686</v>
+      </c>
+      <c r="B6" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>741</v>
+      </c>
+      <c r="B9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>742</v>
+      </c>
+      <c r="B13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>743</v>
+      </c>
+      <c r="B17" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>744</v>
+      </c>
+      <c r="B21" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>745</v>
+      </c>
+      <c r="B25" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>746</v>
+      </c>
+      <c r="B29" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>747</v>
+      </c>
+      <c r="B33" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>748</v>
+      </c>
+      <c r="B39" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>749</v>
+      </c>
+      <c r="B41" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>28</v>
+      </c>
+      <c r="B44" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>750</v>
+      </c>
+      <c r="B45" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>30</v>
+      </c>
+      <c r="B48" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>751</v>
+      </c>
+      <c r="B49" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>32</v>
+      </c>
+      <c r="B52" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>752</v>
+      </c>
+      <c r="B53" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>34</v>
+      </c>
+      <c r="B56" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>753</v>
+      </c>
+      <c r="B57" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>36</v>
+      </c>
+      <c r="B60" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>754</v>
+      </c>
+      <c r="B61" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>718</v>
+      </c>
+      <c r="B64" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>755</v>
+      </c>
+      <c r="B65" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>719</v>
+      </c>
+      <c r="B66" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>756</v>
+      </c>
+      <c r="B67" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>720</v>
+      </c>
+      <c r="B68" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>757</v>
+      </c>
+      <c r="B69" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>721</v>
+      </c>
+      <c r="B70" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>758</v>
+      </c>
+      <c r="B71" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>722</v>
+      </c>
+      <c r="B72" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>759</v>
+      </c>
+      <c r="B73" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>723</v>
+      </c>
+      <c r="B74" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>760</v>
+      </c>
+      <c r="B75" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>8</v>
+      </c>
+      <c r="B83" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>193</v>
+      </c>
+      <c r="B84" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>813</v>
+      </c>
+      <c r="B85" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>194</v>
+      </c>
+      <c r="B86" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>814</v>
+      </c>
+      <c r="B87" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>195</v>
+      </c>
+      <c r="B88" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>815</v>
+      </c>
+      <c r="B89" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>196</v>
+      </c>
+      <c r="B90" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>816</v>
+      </c>
+      <c r="B91" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>198</v>
+      </c>
+      <c r="B92" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>817</v>
+      </c>
+      <c r="B93" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>200</v>
+      </c>
+      <c r="B94" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>818</v>
+      </c>
+      <c r="B95" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>202</v>
+      </c>
+      <c r="B96" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>819</v>
+      </c>
+      <c r="B97" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>204</v>
+      </c>
+      <c r="B98" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>820</v>
+      </c>
+      <c r="B99" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>206</v>
+      </c>
+      <c r="B100" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>821</v>
+      </c>
+      <c r="B101" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>208</v>
+      </c>
+      <c r="B102" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>822</v>
+      </c>
+      <c r="B103" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>210</v>
+      </c>
+      <c r="B104" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>823</v>
+      </c>
+      <c r="B105" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>212</v>
+      </c>
+      <c r="B106" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>824</v>
+      </c>
+      <c r="B107" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>214</v>
+      </c>
+      <c r="B108" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>825</v>
+      </c>
+      <c r="B109" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>216</v>
+      </c>
+      <c r="B110" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>826</v>
+      </c>
+      <c r="B111" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>218</v>
+      </c>
+      <c r="B112" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>827</v>
+      </c>
+      <c r="B113" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>220</v>
+      </c>
+      <c r="B114" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>828</v>
+      </c>
+      <c r="B115" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>829</v>
+      </c>
+      <c r="B116" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>830</v>
+      </c>
+      <c r="B117" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>831</v>
+      </c>
+      <c r="B118" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>832</v>
+      </c>
+      <c r="B119" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>833</v>
+      </c>
+      <c r="B120" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>834</v>
+      </c>
+      <c r="B121" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>835</v>
+      </c>
+      <c r="B122" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>836</v>
+      </c>
+      <c r="B123" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>837</v>
+      </c>
+      <c r="B124" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>838</v>
+      </c>
+      <c r="B125" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>839</v>
+      </c>
+      <c r="B126" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>840</v>
+      </c>
+      <c r="B127" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>841</v>
+      </c>
+      <c r="B128" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>842</v>
+      </c>
+      <c r="B129" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>843</v>
+      </c>
+      <c r="B130" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>844</v>
+      </c>
+      <c r="B131" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>845</v>
+      </c>
+      <c r="B132" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>846</v>
+      </c>
+      <c r="B133" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>847</v>
+      </c>
+      <c r="B134" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>848</v>
+      </c>
+      <c r="B135" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>849</v>
+      </c>
+      <c r="B136" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>850</v>
+      </c>
+      <c r="B137" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>851</v>
+      </c>
+      <c r="B138" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>852</v>
+      </c>
+      <c r="B139" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>853</v>
+      </c>
+      <c r="B140" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>854</v>
+      </c>
+      <c r="B141" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>855</v>
+      </c>
+      <c r="B142" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>856</v>
+      </c>
+      <c r="B143" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>858</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A7ED6AA-780D-40B6-8131-5D17C4E940B1}">
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="90.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>764</v>
+      </c>
+      <c r="B4" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>687</v>
+      </c>
+      <c r="B5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>765</v>
+      </c>
+      <c r="B6" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>766</v>
+      </c>
+      <c r="B7" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>513</v>
+      </c>
+      <c r="B8" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>511</v>
+      </c>
+      <c r="B9" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>767</v>
+      </c>
+      <c r="B10" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>768</v>
+      </c>
+      <c r="B11" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>769</v>
+      </c>
+      <c r="B12" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>770</v>
+      </c>
+      <c r="B13" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>771</v>
+      </c>
+      <c r="B14" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>772</v>
+      </c>
+      <c r="B15" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>773</v>
+      </c>
+      <c r="B16" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>774</v>
+      </c>
+      <c r="B17" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>775</v>
+      </c>
+      <c r="B18" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>776</v>
+      </c>
+      <c r="B19" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>777</v>
+      </c>
+      <c r="B20" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>778</v>
+      </c>
+      <c r="B21" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>779</v>
+      </c>
+      <c r="B22" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>780</v>
+      </c>
+      <c r="B23" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>782</v>
+      </c>
+      <c r="B25" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>783</v>
+      </c>
+      <c r="B26" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>784</v>
+      </c>
+      <c r="B27" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>785</v>
+      </c>
+      <c r="B28" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>786</v>
+      </c>
+      <c r="B29" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>787</v>
+      </c>
+      <c r="B30" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>788</v>
+      </c>
+      <c r="B31" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>789</v>
+      </c>
+      <c r="B32" t="s">
+        <v>806</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FF6723E-FEDE-4F29-9272-6E8BFEC4F8C1}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -8316,6 +10290,7 @@
   <dimension ref="A1:C184"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -9826,10 +11801,11 @@
   </sheetPr>
   <dimension ref="A1:L505"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
   <cols>
@@ -17093,8 +19069,9 @@
       <pane xSplit="1" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="C34" sqref="C34"/>
+      <selection pane="bottomRight" activeCell="D84" sqref="D84"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -18675,10 +20652,11 @@
   </sheetPr>
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F56" sqref="F56"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -20472,6 +22450,99 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68F51FC5-61D6-4D3D-A84E-E413F531C436}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B9"/>
+    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2290</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>762</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2309</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>2311</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2315</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>2312</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2316</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>1482</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2317</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>2313</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2303</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>2314</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2318</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>2297</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2319</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07280A18-1BD1-4FDB-AB03-8EC8E7A45C01}">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
@@ -20479,6 +22550,7 @@
   <dimension ref="A1:A158"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -21280,16 +23352,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F730E738-71E8-4BB9-9BDD-FAFBA3CE3EC3}">
-  <dimension ref="A1:B146"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3487DC-80B1-42DB-B16C-C7930D5F410A}">
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="56.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -21297,1319 +23371,63 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2297</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>191</v>
+        <v>2298</v>
       </c>
       <c r="B3" t="s">
-        <v>762</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>687</v>
+        <v>2299</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>2304</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>685</v>
+        <v>97</v>
       </c>
       <c r="B5" t="s">
-        <v>688</v>
+        <v>2290</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>686</v>
+        <v>2300</v>
       </c>
       <c r="B6" t="s">
-        <v>689</v>
+        <v>2305</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>2301</v>
       </c>
       <c r="B7" t="s">
-        <v>103</v>
+        <v>2306</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>2286</v>
       </c>
       <c r="B8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>741</v>
-      </c>
-      <c r="B9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>742</v>
-      </c>
-      <c r="B13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>743</v>
-      </c>
-      <c r="B17" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>744</v>
-      </c>
-      <c r="B21" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>697</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>18</v>
-      </c>
-      <c r="B24" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>745</v>
-      </c>
-      <c r="B25" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>746</v>
-      </c>
-      <c r="B29" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>22</v>
-      </c>
-      <c r="B32" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>747</v>
-      </c>
-      <c r="B33" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>24</v>
-      </c>
-      <c r="B36" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>748</v>
-      </c>
-      <c r="B39" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>26</v>
-      </c>
-      <c r="B40" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>749</v>
-      </c>
-      <c r="B41" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>28</v>
-      </c>
-      <c r="B44" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>750</v>
-      </c>
-      <c r="B45" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>30</v>
-      </c>
-      <c r="B48" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>751</v>
-      </c>
-      <c r="B49" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>32</v>
-      </c>
-      <c r="B52" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>752</v>
-      </c>
-      <c r="B53" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>34</v>
-      </c>
-      <c r="B56" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>753</v>
-      </c>
-      <c r="B57" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>36</v>
-      </c>
-      <c r="B60" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>754</v>
-      </c>
-      <c r="B61" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
-        <v>718</v>
-      </c>
-      <c r="B64" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>755</v>
-      </c>
-      <c r="B65" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>719</v>
-      </c>
-      <c r="B66" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
-        <v>756</v>
-      </c>
-      <c r="B67" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
-        <v>720</v>
-      </c>
-      <c r="B68" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
-        <v>757</v>
-      </c>
-      <c r="B69" t="s">
-        <v>737</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
-        <v>721</v>
-      </c>
-      <c r="B70" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
-        <v>758</v>
-      </c>
-      <c r="B71" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
-        <v>722</v>
-      </c>
-      <c r="B72" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
-        <v>759</v>
-      </c>
-      <c r="B73" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
-        <v>723</v>
-      </c>
-      <c r="B74" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
-        <v>760</v>
-      </c>
-      <c r="B75" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
-        <v>8</v>
-      </c>
-      <c r="B83" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
-        <v>193</v>
-      </c>
-      <c r="B84" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
-        <v>813</v>
-      </c>
-      <c r="B85" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
-        <v>194</v>
-      </c>
-      <c r="B86" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
-        <v>814</v>
-      </c>
-      <c r="B87" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
-        <v>195</v>
-      </c>
-      <c r="B88" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A89" t="s">
-        <v>815</v>
-      </c>
-      <c r="B89" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A90" t="s">
-        <v>196</v>
-      </c>
-      <c r="B90" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
-        <v>816</v>
-      </c>
-      <c r="B91" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
-        <v>198</v>
-      </c>
-      <c r="B92" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
-        <v>817</v>
-      </c>
-      <c r="B93" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A94" t="s">
-        <v>200</v>
-      </c>
-      <c r="B94" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A95" t="s">
-        <v>818</v>
-      </c>
-      <c r="B95" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A96" t="s">
-        <v>202</v>
-      </c>
-      <c r="B96" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A97" t="s">
-        <v>819</v>
-      </c>
-      <c r="B97" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A98" t="s">
-        <v>204</v>
-      </c>
-      <c r="B98" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A99" t="s">
-        <v>820</v>
-      </c>
-      <c r="B99" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A100" t="s">
-        <v>206</v>
-      </c>
-      <c r="B100" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A101" t="s">
-        <v>821</v>
-      </c>
-      <c r="B101" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A102" t="s">
-        <v>208</v>
-      </c>
-      <c r="B102" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A103" t="s">
-        <v>822</v>
-      </c>
-      <c r="B103" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A104" t="s">
-        <v>210</v>
-      </c>
-      <c r="B104" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A105" t="s">
-        <v>823</v>
-      </c>
-      <c r="B105" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A106" t="s">
-        <v>212</v>
-      </c>
-      <c r="B106" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A107" t="s">
-        <v>824</v>
-      </c>
-      <c r="B107" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A108" t="s">
-        <v>214</v>
-      </c>
-      <c r="B108" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A109" t="s">
-        <v>825</v>
-      </c>
-      <c r="B109" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A110" t="s">
-        <v>216</v>
-      </c>
-      <c r="B110" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A111" t="s">
-        <v>826</v>
-      </c>
-      <c r="B111" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A112" t="s">
-        <v>218</v>
-      </c>
-      <c r="B112" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A113" t="s">
-        <v>827</v>
-      </c>
-      <c r="B113" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A114" t="s">
-        <v>220</v>
-      </c>
-      <c r="B114" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A115" t="s">
-        <v>828</v>
-      </c>
-      <c r="B115" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A116" t="s">
-        <v>829</v>
-      </c>
-      <c r="B116" t="s">
-        <v>859</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A117" t="s">
-        <v>830</v>
-      </c>
-      <c r="B117" t="s">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A118" t="s">
-        <v>831</v>
-      </c>
-      <c r="B118" t="s">
-        <v>861</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A119" t="s">
-        <v>832</v>
-      </c>
-      <c r="B119" t="s">
-        <v>862</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A120" t="s">
-        <v>833</v>
-      </c>
-      <c r="B120" t="s">
-        <v>863</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A121" t="s">
-        <v>834</v>
-      </c>
-      <c r="B121" t="s">
-        <v>864</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A122" t="s">
-        <v>835</v>
-      </c>
-      <c r="B122" t="s">
-        <v>865</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A123" t="s">
-        <v>836</v>
-      </c>
-      <c r="B123" t="s">
-        <v>866</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A124" t="s">
-        <v>837</v>
-      </c>
-      <c r="B124" t="s">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A125" t="s">
-        <v>838</v>
-      </c>
-      <c r="B125" t="s">
-        <v>868</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A126" t="s">
-        <v>839</v>
-      </c>
-      <c r="B126" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A127" t="s">
-        <v>840</v>
-      </c>
-      <c r="B127" t="s">
-        <v>870</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A128" t="s">
-        <v>841</v>
-      </c>
-      <c r="B128" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A129" t="s">
-        <v>842</v>
-      </c>
-      <c r="B129" t="s">
-        <v>872</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A130" t="s">
-        <v>843</v>
-      </c>
-      <c r="B130" t="s">
-        <v>873</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A131" t="s">
-        <v>844</v>
-      </c>
-      <c r="B131" t="s">
-        <v>874</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A132" t="s">
-        <v>845</v>
-      </c>
-      <c r="B132" t="s">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A133" t="s">
-        <v>846</v>
-      </c>
-      <c r="B133" t="s">
-        <v>876</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A134" t="s">
-        <v>847</v>
-      </c>
-      <c r="B134" t="s">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A135" t="s">
-        <v>848</v>
-      </c>
-      <c r="B135" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A136" t="s">
-        <v>849</v>
-      </c>
-      <c r="B136" t="s">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A137" t="s">
-        <v>850</v>
-      </c>
-      <c r="B137" t="s">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A138" t="s">
-        <v>851</v>
-      </c>
-      <c r="B138" t="s">
-        <v>881</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A139" t="s">
-        <v>852</v>
-      </c>
-      <c r="B139" t="s">
-        <v>882</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A140" t="s">
-        <v>853</v>
-      </c>
-      <c r="B140" t="s">
-        <v>883</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A141" t="s">
-        <v>854</v>
-      </c>
-      <c r="B141" t="s">
-        <v>884</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A142" t="s">
-        <v>855</v>
-      </c>
-      <c r="B142" t="s">
-        <v>885</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A143" t="s">
-        <v>856</v>
-      </c>
-      <c r="B143" t="s">
-        <v>886</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A144" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A145" t="s">
-        <v>857</v>
-      </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A146" t="s">
-        <v>858</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A7ED6AA-780D-40B6-8131-5D17C4E940B1}">
-  <dimension ref="A1:B32"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="90.08984375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>764</v>
-      </c>
-      <c r="B4" t="s">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>687</v>
-      </c>
-      <c r="B5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>765</v>
-      </c>
-      <c r="B6" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>766</v>
-      </c>
-      <c r="B7" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>513</v>
-      </c>
-      <c r="B8" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>511</v>
-      </c>
-      <c r="B9" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>767</v>
-      </c>
-      <c r="B10" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>768</v>
-      </c>
-      <c r="B11" t="s">
-        <v>791</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>769</v>
-      </c>
-      <c r="B12" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>770</v>
-      </c>
-      <c r="B13" t="s">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>771</v>
-      </c>
-      <c r="B14" t="s">
-        <v>812</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>772</v>
-      </c>
-      <c r="B15" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>773</v>
-      </c>
-      <c r="B16" t="s">
-        <v>799</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>774</v>
-      </c>
-      <c r="B17" t="s">
-        <v>792</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>775</v>
-      </c>
-      <c r="B18" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>776</v>
-      </c>
-      <c r="B19" t="s">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>777</v>
-      </c>
-      <c r="B20" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>778</v>
-      </c>
-      <c r="B21" t="s">
-        <v>809</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>779</v>
-      </c>
-      <c r="B22" t="s">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>780</v>
-      </c>
-      <c r="B23" t="s">
-        <v>811</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>782</v>
-      </c>
-      <c r="B25" t="s">
-        <v>801</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>783</v>
-      </c>
-      <c r="B26" t="s">
-        <v>804</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>784</v>
-      </c>
-      <c r="B27" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>785</v>
-      </c>
-      <c r="B28" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>786</v>
-      </c>
-      <c r="B29" t="s">
-        <v>793</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>787</v>
-      </c>
-      <c r="B30" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>788</v>
-      </c>
-      <c r="B31" t="s">
-        <v>805</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>789</v>
-      </c>
-      <c r="B32" t="s">
-        <v>806</v>
+        <v>2307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Timestamp correction and longitudinal metabolomics
</commit_message>
<xml_diff>
--- a/data/CABG Hyperglycemia Variable List.xlsx
+++ b/data/CABG Hyperglycemia Variable List.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDA32A2-20D7-4944-AD54-61509A2D8710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B978AC98-631D-48B9-A728-76ED832C453B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-3210" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="5" xr2:uid="{D170740D-F730-4FE0-A2DA-00C8EA3E9EA2}"/>
+    <workbookView xWindow="-16320" yWindow="-15840" windowWidth="16440" windowHeight="28440" firstSheet="19" activeTab="21" xr2:uid="{D170740D-F730-4FE0-A2DA-00C8EA3E9EA2}"/>
   </bookViews>
   <sheets>
     <sheet name="or_to_icu" sheetId="1" state="hidden" r:id="rId1"/>
@@ -27,8 +27,11 @@
     <sheet name="screening_cs" sheetId="17" r:id="rId17"/>
     <sheet name="surgery_cs" sheetId="18" r:id="rId18"/>
     <sheet name="stress hyperglycemia 4 to 24h" sheetId="21" r:id="rId19"/>
-    <sheet name="aha glucose" sheetId="5" state="hidden" r:id="rId20"/>
-    <sheet name="aha patient" sheetId="6" state="hidden" r:id="rId21"/>
+    <sheet name="blood draws timestamps" sheetId="23" r:id="rId20"/>
+    <sheet name="c18_feature_2" sheetId="24" r:id="rId21"/>
+    <sheet name="hilic_feature_2" sheetId="25" r:id="rId22"/>
+    <sheet name="aha glucose" sheetId="5" state="hidden" r:id="rId23"/>
+    <sheet name="aha patient" sheetId="6" state="hidden" r:id="rId24"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'METACABG 20230706'!$B$1:$J$505</definedName>
@@ -89,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6959" uniqueCount="4097">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7057" uniqueCount="4163">
   <si>
     <t>variable</t>
   </si>
@@ -12443,12 +12446,210 @@
   <si>
     <t>dialysis_any</t>
   </si>
+  <si>
+    <t>visit1</t>
+  </si>
+  <si>
+    <t>visit2</t>
+  </si>
+  <si>
+    <t>visit3</t>
+  </si>
+  <si>
+    <t>visit4</t>
+  </si>
+  <si>
+    <t>visit5</t>
+  </si>
+  <si>
+    <t>valid_visit1</t>
+  </si>
+  <si>
+    <t>valid_visit2</t>
+  </si>
+  <si>
+    <t>valid_visit3</t>
+  </si>
+  <si>
+    <t>valid_visit4</t>
+  </si>
+  <si>
+    <t>valid_visit5</t>
+  </si>
+  <si>
+    <t>diff_surgerystartmv1</t>
+  </si>
+  <si>
+    <t>diff_v2msurgerystart</t>
+  </si>
+  <si>
+    <t>diff_v3msurgeryend</t>
+  </si>
+  <si>
+    <t>diff_v4msurgeryend</t>
+  </si>
+  <si>
+    <t>diff_v5msurgeryend</t>
+  </si>
+  <si>
+    <t>flags_v1</t>
+  </si>
+  <si>
+    <t>flags_v2</t>
+  </si>
+  <si>
+    <t>flags_v3</t>
+  </si>
+  <si>
+    <t>flags_v4</t>
+  </si>
+  <si>
+    <t>flags_v5</t>
+  </si>
+  <si>
+    <t>visit1_imputed</t>
+  </si>
+  <si>
+    <t>visit2_imputed</t>
+  </si>
+  <si>
+    <t>visit3_imputed</t>
+  </si>
+  <si>
+    <t>visit4_imputed</t>
+  </si>
+  <si>
+    <t>visit5_imputed</t>
+  </si>
+  <si>
+    <t>Original timestamp for V1</t>
+  </si>
+  <si>
+    <t>Original timestamp for V2</t>
+  </si>
+  <si>
+    <t>Original timestamp for V3</t>
+  </si>
+  <si>
+    <t>Original timestamp for V4</t>
+  </si>
+  <si>
+    <t>Original timestamp for V5</t>
+  </si>
+  <si>
+    <t>Notes for patient ID</t>
+  </si>
+  <si>
+    <t>Was hour == 0 and minute == 0 for visit 1? (Valid, Invalid, Missing Timestamp)</t>
+  </si>
+  <si>
+    <t>Was hour == 0 and minute == 0 for visit 2? (Valid, Invalid, Missing Timestamp)</t>
+  </si>
+  <si>
+    <t>Was hour == 0 and minute == 0 for visit 3? (Valid, Invalid, Missing Timestamp)</t>
+  </si>
+  <si>
+    <t>Was hour == 0 and minute == 0 for visit 4? (Valid, Invalid, Missing Timestamp)</t>
+  </si>
+  <si>
+    <t>Was hour == 0 and minute == 0 for visit 5? (Valid, Invalid, Missing Timestamp)</t>
+  </si>
+  <si>
+    <t>Timestamp for surgery start (from surgery_cs)</t>
+  </si>
+  <si>
+    <t>Timestamp for surgery end (from surgery_cs)</t>
+  </si>
+  <si>
+    <t>If valid_visit1 == "Valid", difference in minutes between surgery start and visit 1</t>
+  </si>
+  <si>
+    <t>If valid_visit5 == "Valid", difference in minutes between surgery end and visit 5</t>
+  </si>
+  <si>
+    <t>If valid_visit4 == "Valid", difference in minutes between surgery end and visit 4</t>
+  </si>
+  <si>
+    <t>If valid_visit3 == "Valid", difference in minutes between surgery end and visit 3</t>
+  </si>
+  <si>
+    <t>If valid_visit2 == "Valid", difference in minutes between visit2 and surgery start</t>
+  </si>
+  <si>
+    <t>Was data collected more than 24 hours ago OR missing OR looks good?</t>
+  </si>
+  <si>
+    <t>Was data collected more than 2 hours later OR missing or looks good?</t>
+  </si>
+  <si>
+    <t>Was data collected more than 48 hours later OR missing or before surgery or before 24 hours or looks good?</t>
+  </si>
+  <si>
+    <t>Was data collected more than 96 hours later OR less than 72 hours later OR missing or looks good?</t>
+  </si>
+  <si>
+    <t>Was data collected more than 30 days later OR missing or looks good?</t>
+  </si>
+  <si>
+    <t>visit1 imputed using median of diff_surgerystartmv1</t>
+  </si>
+  <si>
+    <t>visit2 imputed using median of diff_v2msurgerystart</t>
+  </si>
+  <si>
+    <t>visit3 imputed using median of diff_v3msurgeryend</t>
+  </si>
+  <si>
+    <t>visit4 imputed using median of diff_v4msurgeryend</t>
+  </si>
+  <si>
+    <t>visit5 imputed using median of diff_v5msurgeryend</t>
+  </si>
+  <si>
+    <t>mz</t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>V3</t>
+  </si>
+  <si>
+    <t>V4</t>
+  </si>
+  <si>
+    <t>V5</t>
+  </si>
+  <si>
+    <t>mass to charge ratio</t>
+  </si>
+  <si>
+    <t>retention time</t>
+  </si>
+  <si>
+    <t>Intensity for Visit 1</t>
+  </si>
+  <si>
+    <t>Intensity for Visit 2</t>
+  </si>
+  <si>
+    <t>Intensity for Visit 3</t>
+  </si>
+  <si>
+    <t>Intensity for Visit 4</t>
+  </si>
+  <si>
+    <t>Intensity for Visit 5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -12504,6 +12705,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -14842,7 +15049,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED7BF4C5-AF7C-4E65-B822-62C042B31EF5}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -14914,7 +15123,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ED1AF4F-5AA5-4979-BAAF-416AE60C7B2E}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -15040,6 +15251,449 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5E5E5AE-7933-4ACC-B2DD-A0F04160D626}">
+  <dimension ref="A1:B30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4097</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>4098</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4099</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>4100</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>4101</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>893</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>4102</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>4103</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>4104</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>4105</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>4106</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>547</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>548</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4134</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>4107</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>4108</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>4109</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4138</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>4110</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>4111</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>4112</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4140</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>4113</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4141</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>4114</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4142</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>4115</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4143</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>4116</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4144</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>4117</v>
+      </c>
+      <c r="B26" t="s">
+        <v>4145</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>4118</v>
+      </c>
+      <c r="B27" t="s">
+        <v>4146</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>4119</v>
+      </c>
+      <c r="B28" t="s">
+        <v>4147</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>4120</v>
+      </c>
+      <c r="B29" t="s">
+        <v>4148</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>4121</v>
+      </c>
+      <c r="B30" t="s">
+        <v>4149</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C9AC9E-340B-4C4D-B052-1D6154EDEF7E}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.90625" customWidth="1"/>
+    <col min="2" max="2" width="23.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4150</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1341</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4151</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>4152</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>4153</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>4154</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>4155</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4162</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBF56752-5D5A-4C86-8E0C-0A0A9B1593D1}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.90625" customWidth="1"/>
+    <col min="2" max="2" width="23.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4150</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1341</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4151</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>4152</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>4153</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>4154</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>4155</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4162</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F730E738-71E8-4BB9-9BDD-FAFBA3CE3EC3}">
   <dimension ref="A1:B146"/>
   <sheetViews>
@@ -16110,7 +16764,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A7ED6AA-780D-40B6-8131-5D17C4E940B1}">
   <dimension ref="A1:B32"/>
   <sheetViews>
@@ -27305,8 +27959,8 @@
   </sheetPr>
   <dimension ref="A1:D1385"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A916" workbookViewId="0">
-      <selection activeCell="D941" sqref="D941"/>
+    <sheetView topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="B163" sqref="B163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -28948,12 +29602,18 @@
       <c r="B164" t="s">
         <v>2998</v>
       </c>
+      <c r="C164" t="s">
+        <v>2998</v>
+      </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A165" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B165" t="s">
+        <v>2999</v>
+      </c>
+      <c r="C165" t="s">
         <v>2999</v>
       </c>
       <c r="D165" t="s">

</xml_diff>

<commit_message>
Added data cleaning for mummichog data and removed extra rows from insulindrip_longitudinal
</commit_message>
<xml_diff>
--- a/data/CABG Hyperglycemia Variable List.xlsx
+++ b/data/CABG Hyperglycemia Variable List.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B978AC98-631D-48B9-A728-76ED832C453B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688A11FF-4485-420F-A7FD-E48840B02746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-15840" windowWidth="16440" windowHeight="28440" firstSheet="19" activeTab="21" xr2:uid="{D170740D-F730-4FE0-A2DA-00C8EA3E9EA2}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10360" firstSheet="21" activeTab="23" xr2:uid="{D170740D-F730-4FE0-A2DA-00C8EA3E9EA2}"/>
   </bookViews>
   <sheets>
     <sheet name="or_to_icu" sheetId="1" state="hidden" r:id="rId1"/>
@@ -30,8 +30,10 @@
     <sheet name="blood draws timestamps" sheetId="23" r:id="rId20"/>
     <sheet name="c18_feature_2" sheetId="24" r:id="rId21"/>
     <sheet name="hilic_feature_2" sheetId="25" r:id="rId22"/>
-    <sheet name="aha glucose" sheetId="5" state="hidden" r:id="rId23"/>
-    <sheet name="aha patient" sheetId="6" state="hidden" r:id="rId24"/>
+    <sheet name="C18_Mummichog Metabolite Match" sheetId="26" r:id="rId23"/>
+    <sheet name="HIL_Mummichog Metabolite Match" sheetId="27" r:id="rId24"/>
+    <sheet name="aha glucose" sheetId="5" state="hidden" r:id="rId25"/>
+    <sheet name="aha patient" sheetId="6" state="hidden" r:id="rId26"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'METACABG 20230706'!$B$1:$J$505</definedName>
@@ -92,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7057" uniqueCount="4163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7091" uniqueCount="4177">
   <si>
     <t>variable</t>
   </si>
@@ -12643,6 +12645,48 @@
   </si>
   <si>
     <t>Intensity for Visit 5</t>
+  </si>
+  <si>
+    <t>Compound_ID</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>match_form</t>
+  </si>
+  <si>
+    <t>mz_difference</t>
+  </si>
+  <si>
+    <t>in_pathways</t>
+  </si>
+  <si>
+    <t>evidence_score</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>all_possibles</t>
+  </si>
+  <si>
+    <t>Mummichog Compound ID?</t>
+  </si>
+  <si>
+    <t>Compound Name</t>
+  </si>
+  <si>
+    <t>Input M/Z ratio</t>
+  </si>
+  <si>
+    <t>Form match with adduct</t>
+  </si>
+  <si>
+    <t>Difference in M/Z relative to Compound_ID</t>
+  </si>
+  <si>
+    <t>Which pathways are the Compound present in?</t>
   </si>
 </sst>
 </file>
@@ -15050,7 +15094,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B6"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15606,8 +15650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBF56752-5D5A-4C86-8E0C-0A0A9B1593D1}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15694,6 +15738,186 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D743FB1F-4F45-4EF9-805E-52209AEA1864}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.90625" customWidth="1"/>
+    <col min="2" max="2" width="23.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4163</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4164</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>4150</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4165</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>4166</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>4167</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>4168</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>4169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>4170</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDBEA197-DF25-44D0-9C28-2365EC9D43B8}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.90625" customWidth="1"/>
+    <col min="2" max="2" width="23.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4163</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4164</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>4150</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4165</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>4166</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>4167</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>4168</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>4169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>4170</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F730E738-71E8-4BB9-9BDD-FAFBA3CE3EC3}">
   <dimension ref="A1:B146"/>
   <sheetViews>
@@ -16764,7 +16988,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A7ED6AA-780D-40B6-8131-5D17C4E940B1}">
   <dimension ref="A1:B32"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added variable lists for aki and afib
</commit_message>
<xml_diff>
--- a/data/CABG Hyperglycemia Variable List.xlsx
+++ b/data/CABG Hyperglycemia Variable List.xlsx
@@ -3,9 +3,10 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688A11FF-4485-420F-A7FD-E48840B02746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3DD5F3-D540-4D8B-9921-8E5E35BADFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10360" firstSheet="21" activeTab="23" xr2:uid="{D170740D-F730-4FE0-A2DA-00C8EA3E9EA2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="3" xr2:uid="{D170740D-F730-4FE0-A2DA-00C8EA3E9EA2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="23" activeTab="25" xr2:uid="{18D90FB9-8B94-4B85-AE0C-47B2E521BCF3}"/>
   </bookViews>
   <sheets>
     <sheet name="or_to_icu" sheetId="1" state="hidden" r:id="rId1"/>
@@ -26,14 +27,16 @@
     <sheet name="labtests_longitudinal" sheetId="22" r:id="rId16"/>
     <sheet name="screening_cs" sheetId="17" r:id="rId17"/>
     <sheet name="surgery_cs" sheetId="18" r:id="rId18"/>
-    <sheet name="stress hyperglycemia 4 to 24h" sheetId="21" r:id="rId19"/>
-    <sheet name="blood draws timestamps" sheetId="23" r:id="rId20"/>
-    <sheet name="c18_feature_2" sheetId="24" r:id="rId21"/>
-    <sheet name="hilic_feature_2" sheetId="25" r:id="rId22"/>
-    <sheet name="C18_Mummichog Metabolite Match" sheetId="26" r:id="rId23"/>
-    <sheet name="HIL_Mummichog Metabolite Match" sheetId="27" r:id="rId24"/>
-    <sheet name="aha glucose" sheetId="5" state="hidden" r:id="rId25"/>
-    <sheet name="aha patient" sheetId="6" state="hidden" r:id="rId26"/>
+    <sheet name="afib" sheetId="29" r:id="rId19"/>
+    <sheet name="aki" sheetId="28" r:id="rId20"/>
+    <sheet name="stress hyperglycemia 4 to 24h" sheetId="21" r:id="rId21"/>
+    <sheet name="blood draws timestamps" sheetId="23" r:id="rId22"/>
+    <sheet name="c18_feature_2" sheetId="24" r:id="rId23"/>
+    <sheet name="hilic_feature_2" sheetId="25" r:id="rId24"/>
+    <sheet name="C18_Mummichog Metabolite Match" sheetId="26" r:id="rId25"/>
+    <sheet name="HIL_Mummichog Metabolite Match" sheetId="27" r:id="rId26"/>
+    <sheet name="aha glucose" sheetId="5" state="hidden" r:id="rId27"/>
+    <sheet name="aha patient" sheetId="6" state="hidden" r:id="rId28"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'METACABG 20230706'!$B$1:$J$505</definedName>
@@ -94,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7091" uniqueCount="4177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7143" uniqueCount="4197">
   <si>
     <t>variable</t>
   </si>
@@ -12687,6 +12690,66 @@
   </si>
   <si>
     <t>Which pathways are the Compound present in?</t>
+  </si>
+  <si>
+    <t>baseline_creatinine</t>
+  </si>
+  <si>
+    <t>absolute_change_from_baseline</t>
+  </si>
+  <si>
+    <t>relative_change_from_baseline</t>
+  </si>
+  <si>
+    <t>aki_status</t>
+  </si>
+  <si>
+    <t>Creatinine value</t>
+  </si>
+  <si>
+    <t>Creatinine at baseline</t>
+  </si>
+  <si>
+    <t>Absolute change in creatinine from baseline</t>
+  </si>
+  <si>
+    <t>Relative change in creatinine from baseline</t>
+  </si>
+  <si>
+    <t>AKI if absolute_change_from_baseline &gt;= 0.3 OR relative_change_from_baseline &gt;= 1.5</t>
+  </si>
+  <si>
+    <t>aki</t>
+  </si>
+  <si>
+    <t>stress hyperglycemia 4 to 24h</t>
+  </si>
+  <si>
+    <t>blood draws timestamps</t>
+  </si>
+  <si>
+    <t>c18_feature_2</t>
+  </si>
+  <si>
+    <t>hilic_feature_2</t>
+  </si>
+  <si>
+    <t>C18_Mummichog Metabolite Match</t>
+  </si>
+  <si>
+    <t>HIL_Mummichog Metabolite Match</t>
+  </si>
+  <si>
+    <t>~/preprocessing/chpre04_time to primary outcomes.R</t>
+  </si>
+  <si>
+    <t>~/data/chd04_blood draws.R</t>
+  </si>
+  <si>
+    <t>~/data/chd05_longitudinal metabolomics.R</t>
+  </si>
+  <si>
+    <t>~/data/chd06_mummichog annotated metabolites.R</t>
   </si>
 </sst>
 </file>
@@ -13369,6 +13432,7 @@
   <dimension ref="A1:C95"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -14172,6 +14236,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -14260,6 +14325,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -14340,6 +14406,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -14428,6 +14495,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -14476,6 +14544,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -14565,6 +14634,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -14693,7 +14763,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E501EB67-4E9F-4768-B92B-2D733FABF3F7}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -14806,6 +14879,7 @@
   <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -15096,6 +15170,7 @@
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -15164,11 +15239,14 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ED1AF4F-5AA5-4979-BAAF-416AE60C7B2E}">
-  <dimension ref="A1:B7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F16D22F-A873-47B1-9C06-C81A6E8AFF8D}">
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+    <sheetView workbookViewId="1">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15194,42 +15272,58 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>2875</v>
+        <v>4005</v>
       </c>
       <c r="B3" t="s">
-        <v>2881</v>
+        <v>632</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>2876</v>
+        <v>4088</v>
       </c>
       <c r="B4" t="s">
-        <v>2880</v>
+        <v>633</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>2877</v>
+        <v>659</v>
       </c>
       <c r="B5" t="s">
-        <v>2882</v>
+        <v>634</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>2878</v>
+        <v>4089</v>
       </c>
       <c r="B6" t="s">
-        <v>2883</v>
+        <v>635</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>2879</v>
+        <v>4090</v>
       </c>
       <c r="B7" t="s">
-        <v>2884</v>
+        <v>2467</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>4091</v>
+      </c>
+      <c r="B8" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>4092</v>
+      </c>
+      <c r="B9" t="s">
+        <v>637</v>
       </c>
     </row>
   </sheetData>
@@ -15242,6 +15336,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -15295,12 +15390,181 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C8E738-E237-44B3-A8F1-4CD3AB88ABB2}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+    <sheetView workbookViewId="1">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>621</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4064</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>2165</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4071</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>2976</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>4177</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>4178</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>4179</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4184</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>4180</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4185</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ED1AF4F-5AA5-4979-BAAF-416AE60C7B2E}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>2875</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2881</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>2876</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>2877</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2882</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>2878</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2883</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>2879</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2884</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5E5E5AE-7933-4ACC-B2DD-A0F04160D626}">
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -15554,13 +15818,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C9AC9E-340B-4C4D-B052-1D6154EDEF7E}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B9"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -15646,13 +15911,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBF56752-5D5A-4C86-8E0C-0A0A9B1593D1}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -15737,13 +16003,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D743FB1F-4F45-4EF9-805E-52209AEA1864}">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -15827,13 +16094,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDBEA197-DF25-44D0-9C28-2365EC9D43B8}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -15917,11 +16185,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F730E738-71E8-4BB9-9BDD-FAFBA3CE3EC3}">
   <dimension ref="A1:B146"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -16988,11 +17257,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A7ED6AA-780D-40B6-8131-5D17C4E940B1}">
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -17262,6 +17532,7 @@
   <dimension ref="A1:C184"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -18767,9 +19038,12 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08C9B308-162A-4FA9-98F4-5823503BDBEE}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -18889,6 +19163,70 @@
       </c>
       <c r="C13" t="s">
         <v>2225</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>671</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4193</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>4186</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4193</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>4187</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4193</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>4188</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4194</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>4189</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4195</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>4190</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4195</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>4191</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4196</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>4192</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4196</v>
       </c>
     </row>
   </sheetData>
@@ -18904,6 +19242,7 @@
   <dimension ref="A1:M505"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
   <cols>
@@ -28183,9 +28522,10 @@
   </sheetPr>
   <dimension ref="A1:D1385"/>
   <sheetViews>
-    <sheetView topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="B163" sqref="B163"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -41072,6 +41412,7 @@
   <dimension ref="A2:M63"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -42655,6 +42996,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7:C7"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -44465,6 +44807,7 @@
   <dimension ref="A1:A28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>

<commit_message>
Updated stress_hyperglycemia_def2 in variable list
</commit_message>
<xml_diff>
--- a/data/CABG Hyperglycemia Variable List.xlsx
+++ b/data/CABG Hyperglycemia Variable List.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3DD5F3-D540-4D8B-9921-8E5E35BADFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1385B5C-0657-407E-BC90-214C39F573E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="3" xr2:uid="{D170740D-F730-4FE0-A2DA-00C8EA3E9EA2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="17" activeTab="20" xr2:uid="{D170740D-F730-4FE0-A2DA-00C8EA3E9EA2}"/>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="23" activeTab="25" xr2:uid="{18D90FB9-8B94-4B85-AE0C-47B2E521BCF3}"/>
   </bookViews>
   <sheets>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7143" uniqueCount="4197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7147" uniqueCount="4201">
   <si>
     <t>variable</t>
   </si>
@@ -12750,6 +12750,18 @@
   </si>
   <si>
     <t>~/data/chd06_mummichog annotated metabolites.R</t>
+  </si>
+  <si>
+    <t>stress_hyperglycemia_def2</t>
+  </si>
+  <si>
+    <t>Stress hyperglycemia definition 2 (1: n_bg_ge140 &gt;= 2 OR n_bg_ge180 &gt;= 1, 0: Else)</t>
+  </si>
+  <si>
+    <t>n_bg_ge180</t>
+  </si>
+  <si>
+    <t>Number of POCT blood glucose measurements &gt;= 189 mg/dL</t>
   </si>
 </sst>
 </file>
@@ -15484,10 +15496,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ED1AF4F-5AA5-4979-BAAF-416AE60C7B2E}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C1:H1048576"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -15538,18 +15550,34 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>2878</v>
+        <v>4199</v>
       </c>
       <c r="B6" t="s">
-        <v>2883</v>
+        <v>4200</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>2878</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2883</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>2879</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>2884</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>4197</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4198</v>
       </c>
     </row>
   </sheetData>
@@ -19040,7 +19068,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08C9B308-162A-4FA9-98F4-5823503BDBEE}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
     <sheetView workbookViewId="1"/>

</xml_diff>